<commit_message>
expand Reader() error reporting make indent_forest work properly with all iterators remove trailing blank lines in indent_forest()
</commit_message>
<xml_diff>
--- a/tests/schema/fixtures/bad-headers.xlsx
+++ b/tests/schema/fixtures/bad-headers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28020" windowHeight="17540" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28020" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="Root" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Ones to many row'!$A$1:$A$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Root!$A$1:$B$2</definedName>
   </definedNames>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -527,7 +527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -567,7 +567,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>

</xml_diff>

<commit_message>
adding test for fuzzy worksheet name matching
</commit_message>
<xml_diff>
--- a/tests/schema/fixtures/bad-headers.xlsx
+++ b/tests/schema/fixtures/bad-headers.xlsx
@@ -5,23 +5,27 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Root" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Main root" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Nodes" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Leaves" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="One to many rows" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Leaves!$A$1:$F$7</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Main root'!$A$1:$B$2</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Nodes!$A$1:$D$4</definedName>
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'One to many rows'!$A$1:$A$13</definedName>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Root!$A$1:$B$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Root!$A$1:$B$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Main root'!$A$1:$B$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Main root'!$A$1:$B$2</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Nodes!$A$1:$D$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">Nodes!$A$1:$D$4</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Leaves!$A$1:$F$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">Leaves!$A$1:$F$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'One to many rows'!$A$1:$A$13</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">'One to many rows'!$A$1:$A$13</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -365,7 +369,7 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -684,7 +688,7 @@
   </sheetPr>
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>

</xml_diff>

<commit_message>
adding inexact attribute name matching, adding case-insensitive worksheet and attribute name matching, adding utility function to get attribute by name which case-insensitive option
</commit_message>
<xml_diff>
--- a/tests/schema/fixtures/bad-headers.xlsx
+++ b/tests/schema/fixtures/bad-headers.xlsx
@@ -20,12 +20,16 @@
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'One to many rows'!$A$1:$A$13</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Main root'!$A$1:$B$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Main root'!$A$1:$B$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Main root'!$A$1:$B$2</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Nodes!$A$1:$D$4</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">Nodes!$A$1:$D$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Nodes!$A$1:$D$4</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Leaves!$A$1:$F$7</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">Leaves!$A$1:$F$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Leaves!$A$1:$F$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'One to many rows'!$A$1:$A$13</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">'One to many rows'!$A$1:$A$13</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'One to many rows'!$A$1:$A$13</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -37,21 +41,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
+  <si>
+    <t>Identifier</t>
+  </si>
+  <si>
+    <t>root</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>€</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
   <si>
     <t>Id</t>
-  </si>
-  <si>
-    <t>root</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>€</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
   <si>
     <t>Root</t>
@@ -374,7 +381,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -438,24 +445,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -469,7 +476,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
@@ -483,7 +490,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
@@ -530,30 +537,30 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>7</v>
@@ -562,18 +569,18 @@
         <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>9</v>
@@ -582,18 +589,18 @@
         <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>11</v>
@@ -602,18 +609,18 @@
         <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>13</v>
@@ -622,18 +629,18 @@
         <v>14</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>15</v>
@@ -642,18 +649,18 @@
         <v>16</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>17</v>
@@ -662,10 +669,10 @@
         <v>18</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -703,67 +710,67 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>